<commit_message>
Conversion of functions to classes
</commit_message>
<xml_diff>
--- a/database/initial_files/data.xlsx
+++ b/database/initial_files/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisb\Desktop\RMS\database\initial_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisb\Desktop\PROJETOS\RMS\database\initial_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E106053-D595-400B-B464-BB2A5127F370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE7F5F3B-CCD1-4935-9CC6-AE18BA5229D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5805" yWindow="-21720" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tables" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
   <si>
     <t>capacity</t>
   </si>
@@ -74,6 +74,18 @@
   </si>
   <si>
     <t>Chicken breast</t>
+  </si>
+  <si>
+    <t>cost</t>
+  </si>
+  <si>
+    <t>0.6</t>
+  </si>
+  <si>
+    <t>0.7</t>
+  </si>
+  <si>
+    <t>2.5</t>
   </si>
 </sst>
 </file>
@@ -394,12 +406,16 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -407,7 +423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10</v>
       </c>
@@ -415,7 +431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>10</v>
       </c>
@@ -423,7 +439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>10</v>
       </c>
@@ -431,7 +447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
@@ -439,7 +455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -447,7 +463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -455,7 +471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -463,7 +479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
@@ -471,7 +487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2</v>
       </c>
@@ -486,18 +502,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ED1CE3B-CF1A-420B-BE25-DC2D68026C69}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -510,8 +527,11 @@
       <c r="D1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -524,8 +544,11 @@
       <c r="D2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -538,8 +561,11 @@
       <c r="D3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -552,8 +578,11 @@
       <c r="D4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -566,8 +595,11 @@
       <c r="D5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -580,8 +612,11 @@
       <c r="D6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -594,8 +629,11 @@
       <c r="D7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -608,8 +646,11 @@
       <c r="D8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -621,6 +662,9 @@
       </c>
       <c r="D9">
         <v>1</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>